<commit_message>
Handle non-numerical input: choose empty_result, positive_result and negative_result (default respectively '', 1 and '')
</commit_message>
<xml_diff>
--- a/lab_results/more_Labresults_clinic_view.xlsx
+++ b/lab_results/more_Labresults_clinic_view.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidelegacci/coding/python/tabecks/git/lab_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidelegacci/coding/python/tabecks/git/lab_tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2824D60A-C0C4-E044-862C-E3D3A3D655BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FF9A11-8DB5-2C45-BD8B-A5A82682DCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="87">
   <si>
     <t>Parameter</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -648,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1199,7 +1205,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>15</v>
@@ -1213,7 +1219,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>15</v>
@@ -1227,7 +1233,7 @@
         <v>14</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>15</v>

</xml_diff>